<commit_message>
add gender to doctors in import
</commit_message>
<xml_diff>
--- a/sql/doctors.xlsx
+++ b/sql/doctors.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>نور باهر حامد عبدالواحد</t>
   </si>
@@ -48,13 +48,16 @@
     <t>baherhamed613@tebah.com</t>
   </si>
   <si>
-    <t>homeTel</t>
-  </si>
-  <si>
     <t>nameAr</t>
   </si>
   <si>
     <t>nameEn</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>male</t>
   </si>
 </sst>
 </file>
@@ -402,7 +405,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -415,28 +418,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -447,22 +450,22 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>123</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>10026276133</v>
-      </c>
-      <c r="H2">
-        <v>404474444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>